<commit_message>
delete old user.db and login sign-in func, update login and sign-in function
</commit_message>
<xml_diff>
--- a/Users_db.xlsx
+++ b/Users_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\Documents\לימודים\שנה ב\Stark_Industries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Desktop\new project\Stark_Industries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CC060B-A65B-496D-999F-3D9522542547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C35E40-FF33-4D25-9C55-8B8784441708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13815" yWindow="3885" windowWidth="14685" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>User type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ID</t>
   </si>
@@ -31,10 +28,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>aaaa</t>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -45,7 +39,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -85,11 +79,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -98,6 +89,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,70 +437,74 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>311369318</v>
+      </c>
+      <c r="B2" s="1">
+        <v>111111</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>123456798</v>
+      </c>
+      <c r="B3" s="1">
+        <v>222222</v>
+      </c>
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>111111</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>456789123</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3333</v>
+      </c>
+      <c r="C4" s="3">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D4" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>222222</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3333</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1234</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>321456987</v>
+      </c>
+      <c r="B5" s="3">
         <v>44444</v>
       </c>
-      <c r="C5" s="4">
-        <v>44444</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add from menu return to login screen
</commit_message>
<xml_diff>
--- a/Users_db.xlsx
+++ b/Users_db.xlsx
@@ -410,7 +410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -521,6 +521,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>123853472</v>
+      </c>
+      <c r="B9" t="n">
+        <v>123</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>124578963</v>
+      </c>
+      <c r="B10" t="n">
+        <v>123</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
add to login and signup function update to player_db
</commit_message>
<xml_diff>
--- a/Users_db.xlsx
+++ b/Users_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\Documents\לימודים\שנה ב\Stark_Industries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Desktop\update project\Stark_Industries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71DD64B-D817-41AF-B6C4-38543A186D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC04C37E-C030-4E5A-9D58-99ACECD9A05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="3810" windowWidth="14685" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -431,19 +431,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C25" sqref="A8:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>311369318</v>
       </c>
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>123456798</v>
       </c>
@@ -475,11 +475,11 @@
         <v>222222</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>456789123</v>
       </c>
@@ -491,92 +491,37 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>321456987</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>44444</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>258741359</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>15478</v>
+        <v>1</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>123852146</v>
-      </c>
       <c r="B7">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>125478524</v>
-      </c>
-      <c r="B8">
-        <v>123</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>123853472</v>
-      </c>
-      <c r="B9">
-        <v>123</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>124578963</v>
-      </c>
-      <c r="B10">
-        <v>123</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>111111111</v>
-      </c>
-      <c r="B11">
-        <v>1234</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>123456789</v>
-      </c>
-      <c r="B12">
-        <v>123456789</v>
-      </c>
-      <c r="C12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding unit tests and updating instructions
</commit_message>
<xml_diff>
--- a/Users_db.xlsx
+++ b/Users_db.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Desktop\update project\Stark_Industries\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC04C37E-C030-4E5A-9D58-99ACECD9A05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="3810" windowWidth="14685" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -34,12 +28,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -79,19 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -99,14 +92,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -153,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,27 +170,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,24 +204,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,103 +379,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="A8:C25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>311369318</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2">
         <v>111111</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>123456798</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3">
         <v>222222</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>456789123</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4">
         <v>3333</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4">
         <v>3</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update game and sign up
</commit_message>
<xml_diff>
--- a/Users_db.xlsx
+++ b/Users_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit9530\Desktop\17.1\Stark_Industries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\Documents\לימודים\שנה ב\Stark_Industries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB51E4D-DAD4-4533-8F07-24D094D09C5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14F7133-7892-4DF4-B1B2-0F5EC96F426F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2655" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,22 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Unnamed: 0</t>
-  </si>
-  <si>
-    <t>Unnamed: 0.1</t>
-  </si>
-  <si>
-    <t>Unnamed: 0.1.1</t>
-  </si>
-  <si>
-    <t>Unnamed: 0.1.1.1</t>
-  </si>
-  <si>
-    <t>Unnamed: 0.1.1.1.1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ID</t>
   </si>
@@ -75,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -98,13 +83,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -409,16 +406,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,168 +428,116 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>311369318</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>111111</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>311369318</v>
-      </c>
-      <c r="H2">
-        <v>111111</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>123456798</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>222222</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>123456798</v>
-      </c>
-      <c r="H3">
-        <v>222222</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>456789123</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3333</v>
       </c>
       <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>456789123</v>
-      </c>
-      <c r="H4">
-        <v>3333</v>
-      </c>
-      <c r="I4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>222222222</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1111</v>
       </c>
       <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>111111111</v>
-      </c>
-      <c r="H5">
-        <v>1111</v>
-      </c>
-      <c r="I5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>157891101</v>
       </c>
-      <c r="H6">
+      <c r="C6">
         <v>123</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>101198751</v>
       </c>
-      <c r="H7">
+      <c r="C7">
         <v>111</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>15</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>123456789</v>
+      </c>
+      <c r="C9">
+        <v>12345</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
     </row>

</xml_diff>